<commit_message>
itcrm con todos los paises
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Yami/ALL COUNTRIES/ponderadores_exportaciones_santa_fe_wide_2001_2024.xlsx
+++ b/Archivos de trabajo/Yami/ALL COUNTRIES/ponderadores_exportaciones_santa_fe_wide_2001_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd03ae9016654ccc/Escritorio/Paper-ITCRM.SF/Archivos de trabajo/Yami/ALL COUNTRIES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_732D5ECB8F79A8D366075C52F37BD2723AC77DBF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C86485F9-4FD2-4319-A554-2F51D45CA49B}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_732D5ECB8F79A8D366075C52F37BD2723AC77DBF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B50E8E5-13A3-4B23-836E-41CC12F0D7EE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1768,7 +1768,10 @@
   <dimension ref="A1:GY30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:XFD27"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="EZ4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="FK9" sqref="FK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>